<commit_message>
added plot for speed vs target speed
</commit_message>
<xml_diff>
--- a/project/excel/speedAndUtilizationResults_zync7000.xlsx
+++ b/project/excel/speedAndUtilizationResults_zync7000.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Luts as logic</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Logic delay</t>
+  </si>
+  <si>
+    <t>Fmax</t>
   </si>
 </sst>
 </file>
@@ -305,11 +308,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="217821648"/>
-        <c:axId val="218182184"/>
+        <c:axId val="149737640"/>
+        <c:axId val="149738032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="217821648"/>
+        <c:axId val="149737640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -366,7 +369,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218182184"/>
+        <c:crossAx val="149738032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -429,7 +432,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218182184"/>
+        <c:axId val="149738032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -486,7 +489,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217821648"/>
+        <c:crossAx val="149737640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -824,11 +827,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="217358024"/>
-        <c:axId val="217824784"/>
+        <c:axId val="149738816"/>
+        <c:axId val="149739208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="217358024"/>
+        <c:axId val="149738816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -885,7 +888,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217824784"/>
+        <c:crossAx val="149739208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -948,7 +951,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="217824784"/>
+        <c:axId val="149739208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1005,7 +1008,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217358024"/>
+        <c:crossAx val="149738816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1144,6 +1147,483 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nb-NO"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Target vs max Frequency</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$B$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fmax</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ark1'!$A$44:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>102000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>105000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ark1'!$B$44:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>50520359.704961106</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50482104.094098635</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64061499.03907752</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82363276.960245982</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>101409593.34753066</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>104297891.13754232</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>104626483.45406896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="149323392"/>
+        <c:axId val="149323784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="149323392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="149323784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+            <c:tx>
+              <c:rich>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="nb-NO"/>
+                    <a:t>Target Frequency [MHz]</a:t>
+                  </a:r>
+                </a:p>
+              </c:rich>
+            </c:tx>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nb-NO"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="149323784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="149323392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+            <c:tx>
+              <c:rich>
+                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="nb-NO"/>
+                    <a:t>Max</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="nb-NO" baseline="0"/>
+                    <a:t> frequency [MHz]</a:t>
+                  </a:r>
+                  <a:endParaRPr lang="nb-NO"/>
+                </a:p>
+              </c:rich>
+            </c:tx>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nb-NO"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nb-NO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1224,6 +1704,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1741,6 +2261,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2313,6 +3349,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagram 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2584,10 +3650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,7 +3664,7 @@
     <col min="9" max="9" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2632,8 +3698,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -2642,7 +3711,7 @@
         <v>100</v>
       </c>
       <c r="C2">
-        <f>( 1 / (2*A2*10^6) ) * 10 ^ 9</f>
+        <f t="shared" ref="C2:C8" si="0">( 1 / (2*A2*10^6) ) * 10 ^ 9</f>
         <v>50</v>
       </c>
       <c r="D2">
@@ -2671,17 +3740,21 @@
         <f>I2-J2</f>
         <v>6.4030000000000022</v>
       </c>
+      <c r="L2">
+        <f>1/( (B2-G2) * 10 ^-9 )</f>
+        <v>50520359.704961106</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>25</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B9" si="0">C3*2</f>
+        <f t="shared" ref="B3:B8" si="1">C3*2</f>
         <v>40</v>
       </c>
       <c r="C3">
-        <f>( 1 / (2*A3*10^6) ) * 10 ^ 9</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="D3">
@@ -2691,7 +3764,7 @@
         <v>1498</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F8" si="1">D3+E3</f>
+        <f t="shared" ref="F3:F8" si="2">D3+E3</f>
         <v>2818</v>
       </c>
       <c r="G3">
@@ -2707,20 +3780,24 @@
         <v>13.032</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K8" si="2">I3-J3</f>
+        <f t="shared" ref="K3:K8" si="3">I3-J3</f>
         <v>6.3900000000000006</v>
       </c>
+      <c r="L3">
+        <f>1/( (B3-G3) * 10 ^-9 )</f>
+        <v>50482104.094098635</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50</v>
       </c>
       <c r="B4">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C4">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="C4">
-        <f>( 1 / (2*A4*10^6) ) * 10 ^ 9</f>
         <v>10</v>
       </c>
       <c r="D4">
@@ -2730,7 +3807,7 @@
         <v>1502</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2822</v>
       </c>
       <c r="G4">
@@ -2746,20 +3823,24 @@
         <v>9.0139999999999993</v>
       </c>
       <c r="K4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.5550000000000015</v>
       </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L8" si="4">1/( (B4-G4) * 10 ^-9 )</f>
+        <v>64061499.03907752</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>75</v>
       </c>
       <c r="B5">
+        <f t="shared" si="1"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="C5">
         <f t="shared" si="0"/>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="C5">
-        <f>( 1 / (2*A5*10^6) ) * 10 ^ 9</f>
         <v>6.666666666666667</v>
       </c>
       <c r="D5">
@@ -2769,7 +3850,7 @@
         <v>1501</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2821</v>
       </c>
       <c r="G5">
@@ -2785,20 +3866,24 @@
         <v>5.3780000000000001</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.3610000000000007</v>
       </c>
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>82363276.960245982</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>100</v>
       </c>
       <c r="B6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C6">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <f>( 1 / (2*A6*10^6) ) * 10 ^ 9</f>
         <v>5</v>
       </c>
       <c r="D6">
@@ -2808,7 +3893,7 @@
         <v>1504</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2824</v>
       </c>
       <c r="G6">
@@ -2824,20 +3909,24 @@
         <v>3.99</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.504999999999999</v>
       </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>101409593.34753066</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>102</v>
       </c>
       <c r="B7">
+        <f t="shared" si="1"/>
+        <v>9.8039215686274517</v>
+      </c>
+      <c r="C7">
         <f t="shared" si="0"/>
-        <v>9.8039215686274517</v>
-      </c>
-      <c r="C7">
-        <f>( 1 / (2*A7*10^6) ) * 10 ^ 9</f>
         <v>4.9019607843137258</v>
       </c>
       <c r="D7">
@@ -2847,7 +3936,7 @@
         <v>1502</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2822</v>
       </c>
       <c r="G7">
@@ -2863,20 +3952,24 @@
         <v>3.242</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.2770000000000001</v>
       </c>
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>104297891.13754232</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>105</v>
       </c>
       <c r="B8">
+        <f t="shared" si="1"/>
+        <v>9.5238095238095237</v>
+      </c>
+      <c r="C8">
         <f t="shared" si="0"/>
-        <v>9.5238095238095237</v>
-      </c>
-      <c r="C8">
-        <f>( 1 / (2*A8*10^6) ) * 10 ^ 9</f>
         <v>4.7619047619047619</v>
       </c>
       <c r="D8">
@@ -2886,7 +3979,7 @@
         <v>1505</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2825</v>
       </c>
       <c r="G8">
@@ -2902,11 +3995,15 @@
         <v>3.09</v>
       </c>
       <c r="K8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.3979999999999997</v>
       </c>
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>104626483.45406896</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2914,7 +4011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10000000</v>
       </c>
@@ -2922,7 +4019,7 @@
         <v>2817</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>25000000</v>
       </c>
@@ -2930,7 +4027,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>50000000</v>
       </c>
@@ -2938,7 +4035,7 @@
         <v>2822</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>75000000</v>
       </c>
@@ -2999,11 +4096,11 @@
         <v>25000000</v>
       </c>
       <c r="B29">
-        <f t="shared" ref="B29:B34" si="3">J3*100</f>
+        <f t="shared" ref="B29:B34" si="5">J3*100</f>
         <v>1303.2</v>
       </c>
       <c r="C29">
-        <f t="shared" ref="C29:C34" si="4">K3*100</f>
+        <f t="shared" ref="C29:C34" si="6">K3*100</f>
         <v>639</v>
       </c>
     </row>
@@ -3012,11 +4109,11 @@
         <v>50000000</v>
       </c>
       <c r="B30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>901.4</v>
       </c>
       <c r="C30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>655.50000000000011</v>
       </c>
     </row>
@@ -3025,11 +4122,11 @@
         <v>75000000</v>
       </c>
       <c r="B31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>537.79999999999995</v>
       </c>
       <c r="C31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>636.1</v>
       </c>
     </row>
@@ -3038,11 +4135,11 @@
         <v>100000000</v>
       </c>
       <c r="B32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>399</v>
       </c>
       <c r="C32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>550.49999999999989</v>
       </c>
     </row>
@@ -3051,11 +4148,11 @@
         <v>102000000</v>
       </c>
       <c r="B33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>324.2</v>
       </c>
       <c r="C33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>627.70000000000005</v>
       </c>
     </row>
@@ -3064,12 +4161,76 @@
         <v>105000000</v>
       </c>
       <c r="B34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>309</v>
       </c>
       <c r="C34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>639.79999999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="B44">
+        <v>50520359.704961106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>25000000</v>
+      </c>
+      <c r="B45">
+        <v>50482104.094098635</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>50000000</v>
+      </c>
+      <c r="B46">
+        <v>64061499.03907752</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>75000000</v>
+      </c>
+      <c r="B47">
+        <v>82363276.960245982</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>100000000</v>
+      </c>
+      <c r="B48">
+        <v>101409593.34753066</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>102000000</v>
+      </c>
+      <c r="B49">
+        <v>104297891.13754232</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>105000000</v>
+      </c>
+      <c r="B50">
+        <v>104626483.45406896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated speedAndUlilization results file. Added csv file for appendix
</commit_message>
<xml_diff>
--- a/project/excel/speedAndUtilizationResults_zync7000.xlsx
+++ b/project/excel/speedAndUtilizationResults_zync7000.xlsx
@@ -308,11 +308,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149737640"/>
-        <c:axId val="149738032"/>
+        <c:axId val="235732080"/>
+        <c:axId val="235732472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149737640"/>
+        <c:axId val="235732080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -369,7 +369,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149738032"/>
+        <c:crossAx val="235732472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -432,7 +432,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149738032"/>
+        <c:axId val="235732472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -489,7 +489,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149737640"/>
+        <c:crossAx val="235732080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -827,11 +827,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149738816"/>
-        <c:axId val="149739208"/>
+        <c:axId val="235734824"/>
+        <c:axId val="235735216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149738816"/>
+        <c:axId val="235734824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -888,7 +888,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149739208"/>
+        <c:crossAx val="235735216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -951,7 +951,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149739208"/>
+        <c:axId val="235735216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1008,7 +1008,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149738816"/>
+        <c:crossAx val="235734824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1187,7 +1187,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1331,11 +1330,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149323392"/>
-        <c:axId val="149323784"/>
+        <c:axId val="235734432"/>
+        <c:axId val="235734040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149323392"/>
+        <c:axId val="235734432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1392,13 +1391,12 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149323784"/>
+        <c:crossAx val="235734040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
-            <c:layout/>
             <c:tx>
               <c:rich>
                 <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -1455,7 +1453,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149323784"/>
+        <c:axId val="235734040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,13 +1510,12 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149323392"/>
+        <c:crossAx val="235734432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
-            <c:layout/>
             <c:tx>
               <c:rich>
                 <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -3652,8 +3649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>